<commit_message>
Additional Import data + New excel sheet
</commit_message>
<xml_diff>
--- a/static/import-data.xlsx
+++ b/static/import-data.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding Projects\For-Chingz\automated-student-attendance-system-fyp\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\Telegram Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D518C68C-8BC8-4BB1-8747-70C32012C685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0029A1EB-81B5-422A-8B18-D788A47C57E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9C40E5B0-304B-4CC1-A5F4-2B3642BC9FA8}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="4" xr2:uid="{9C40E5B0-304B-4CC1-A5F4-2B3642BC9FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Import Users" sheetId="1" r:id="rId1"/>
-    <sheet name="Import Venues" sheetId="2" r:id="rId2"/>
-    <sheet name="Import Courses" sheetId="6" r:id="rId3"/>
-    <sheet name="Assign Courses" sheetId="3" r:id="rId4"/>
-    <sheet name="Import Classes" sheetId="5" r:id="rId5"/>
+    <sheet name="Import Semesters" sheetId="7" r:id="rId2"/>
+    <sheet name="Import Venues" sheetId="2" r:id="rId3"/>
+    <sheet name="Import Courses" sheetId="6" r:id="rId4"/>
+    <sheet name="Assign Courses" sheetId="3" r:id="rId5"/>
+    <sheet name="Import Classes" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="41">
   <si>
     <t>Email</t>
   </si>
@@ -115,45 +116,12 @@
     <t>student</t>
   </si>
   <si>
-    <t>Alice</t>
-  </si>
-  <si>
     <t>female</t>
   </si>
   <si>
-    <t>alice.cock@gmail.com</t>
-  </si>
-  <si>
-    <t>6516 6381</t>
-  </si>
-  <si>
-    <t>pissword</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>bob.ross@gmail.com</t>
-  </si>
-  <si>
-    <t>1242 23542</t>
-  </si>
-  <si>
-    <t>213 12414</t>
-  </si>
-  <si>
     <t>MPSH</t>
   </si>
   <si>
-    <t>MPSH 2</t>
-  </si>
-  <si>
-    <t>MPSH 3</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
     <t>MT301</t>
   </si>
   <si>
@@ -163,53 +131,68 @@
     <t>Speak your mother language</t>
   </si>
   <si>
-    <t>MT302</t>
-  </si>
-  <si>
-    <t>Speak your mother language better</t>
-  </si>
-  <si>
     <t>2026-1</t>
   </si>
   <si>
-    <t>2026-3</t>
-  </si>
-  <si>
-    <t>Higher Mother Tongue</t>
-  </si>
-  <si>
-    <t>MT303</t>
-  </si>
-  <si>
-    <t>Bestest mother language</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>jane.doe@gmail.com</t>
-  </si>
-  <si>
-    <t>3425646 357</t>
-  </si>
-  <si>
-    <t>pissword2</t>
-  </si>
-  <si>
-    <t>bob.me@gmail.com</t>
-  </si>
-  <si>
-    <t>other</t>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Goh Ching Fong</t>
+  </si>
+  <si>
+    <t>gcf@prom.com</t>
+  </si>
+  <si>
+    <t>Hannah Wu</t>
+  </si>
+  <si>
+    <t>hw@prom.com</t>
+  </si>
+  <si>
+    <t>Aaron Bernardo</t>
+  </si>
+  <si>
+    <t>ab@prom.com</t>
+  </si>
+  <si>
+    <t>Chong Ye Han</t>
+  </si>
+  <si>
+    <t>cyh@prom.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -235,8 +218,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -255,9 +244,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -295,7 +284,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -401,7 +390,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -543,7 +532,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -553,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88E5869-6E6D-4388-8D3A-D20B2CDCC9A3}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,25 +581,25 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -619,22 +608,22 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3">
+        <v>12341234</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -642,22 +631,22 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C4">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" t="s">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4">
+        <v>12341234</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -665,19 +654,22 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5">
+        <v>12341234</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -685,22 +677,22 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>12341234</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -710,11 +702,54 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489D4659-D793-44A8-9FC9-3F6CDF401919}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5">
+        <v>46023</v>
+      </c>
+      <c r="C2" s="5">
+        <v>46113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3F7B5E-784E-4B28-83A7-8D139B4DAF00}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,29 +763,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4">
         <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -758,12 +775,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDEBB779-597B-4562-B2F8-5E39177C024E}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,41 +806,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4">
+      <c r="A2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4">
         <v>4</v>
       </c>
     </row>
@@ -832,12 +824,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1E768B-7BC4-4E51-AC68-45A197BBF7A2}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,45 +855,68 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>43</v>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C19B943-F96D-4CF5-82A2-22D9FD42D583}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +926,7 @@
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -936,16 +951,106 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1">
+        <v>46375.5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>46375.625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1">
+        <v>46376</v>
+      </c>
+      <c r="F3" s="2">
+        <v>46376.625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1">
+        <v>46377</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46377.625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1">
+        <v>46378</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46378.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1">
+        <v>46379</v>
+      </c>
+      <c r="F6" s="2">
+        <v>46379.625</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>